<commit_message>
Primeira versão do jogo
</commit_message>
<xml_diff>
--- a/Projetos/Desenvolvimento de Jogos - DJS/planejamento - DJS.xlsx
+++ b/Projetos/Desenvolvimento de Jogos - DJS/planejamento - DJS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>Descrição</t>
   </si>
@@ -74,9 +74,6 @@
   </si>
   <si>
     <t>Testes e correção de bugs. Ajustar o balanceamento do jogo</t>
-  </si>
-  <si>
-    <t>Demonstrar o jogo ao grupo. Discutir melhorias.</t>
   </si>
   <si>
     <t>Desenvolver o jogo</t>
@@ -94,47 +91,41 @@
     <t>22/4/2025</t>
   </si>
   <si>
+    <t>RESPONSÁVEL</t>
+  </si>
+  <si>
+    <t>DATA</t>
+  </si>
+  <si>
+    <t>TAREFAS</t>
+  </si>
+  <si>
+    <t>OK?</t>
+  </si>
+  <si>
+    <t>Definir conceitos do jogo e plataforma</t>
+  </si>
+  <si>
+    <t>//2025</t>
+  </si>
+  <si>
+    <t>/2025</t>
+  </si>
+  <si>
+    <t>Criar Menus</t>
+  </si>
+  <si>
+    <t>Demonstrar o jogo ao grupo e disponibilizar a todos. Discutir melhorias.</t>
+  </si>
+  <si>
     <t>Criar um guia de passo a passo do desenvolvimento do projeto. Mostrar os conceitos aprendidos, junto com os pontos que achou fácil e difícil.
-Mostrar todas as ferramentas utilizadas</t>
-  </si>
-  <si>
-    <t>RESPONSÁVEL</t>
-  </si>
-  <si>
-    <t>DATA</t>
-  </si>
-  <si>
-    <t>TAREFAS</t>
-  </si>
-  <si>
-    <t>OK?</t>
-  </si>
-  <si>
-    <t>Definir conceitos do jogo e plataforma</t>
-  </si>
-  <si>
-    <t>//2025</t>
-  </si>
-  <si>
-    <t>/2025</t>
-  </si>
-  <si>
-    <t>MVP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       Criar um protótipo básico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       Implementar movimentação e mecânica dos componentes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       Criar assets </t>
-  </si>
-  <si>
-    <t xml:space="preserve">       Melhorias</t>
-  </si>
-  <si>
-    <t>Criar Menus</t>
+Mostrar todas as ferramentas utilizadas.</t>
+  </si>
+  <si>
+    <t>Final de Nov</t>
+  </si>
+  <si>
+    <t>Melhorias</t>
   </si>
 </sst>
 </file>
@@ -223,7 +214,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -260,8 +251,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -327,43 +324,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="10" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -380,38 +399,33 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="29">
     <dxf>
       <fill>
         <patternFill>
@@ -446,6 +460,50 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF34A853"/>
+          <bgColor rgb="FF34A853"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF34A853"/>
+          <bgColor rgb="FF34A853"/>
         </patternFill>
       </fill>
     </dxf>
@@ -595,23 +653,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$14" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$15" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$10" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$11" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$8" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -627,23 +673,23 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$8" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$9" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$9" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$7" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$12" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$10" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$7" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$11" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$13" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$12" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -653,15 +699,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>280621</xdr:colOff>
+          <xdr:colOff>276225</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>65943</xdr:rowOff>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>528271</xdr:colOff>
+          <xdr:colOff>523875</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>336306</xdr:rowOff>
+          <xdr:rowOff>333375</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -717,15 +763,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>265967</xdr:colOff>
+          <xdr:colOff>266700</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>197827</xdr:rowOff>
+          <xdr:rowOff>200025</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>485042</xdr:colOff>
+          <xdr:colOff>485775</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>359752</xdr:rowOff>
+          <xdr:rowOff>361950</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -781,15 +827,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>286207</xdr:colOff>
+          <xdr:colOff>285750</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>2565</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>476707</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>12090</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -845,15 +891,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>298114</xdr:colOff>
+          <xdr:colOff>295275</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>10899</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>488614</xdr:colOff>
+          <xdr:colOff>485775</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>1374</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -909,143 +955,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>289779</xdr:colOff>
-          <xdr:row>7</xdr:row>
-          <xdr:rowOff>23996</xdr:rowOff>
+          <xdr:colOff>295275</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>499329</xdr:colOff>
-          <xdr:row>7</xdr:row>
-          <xdr:rowOff>223106</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1041" name="Check Box 17" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1041"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>299304</xdr:colOff>
+          <xdr:colOff>495300</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>15661</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>489804</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>213304</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1042" name="Check Box 18" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1042"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>293352</xdr:colOff>
-          <xdr:row>11</xdr:row>
-          <xdr:rowOff>31139</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>493377</xdr:colOff>
-          <xdr:row>11</xdr:row>
-          <xdr:rowOff>209732</xdr:rowOff>
+          <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1101,15 +1019,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>289780</xdr:colOff>
+          <xdr:colOff>285750</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>35902</xdr:rowOff>
+          <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>480280</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>216877</xdr:rowOff>
+          <xdr:rowOff>219075</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1165,15 +1083,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>287398</xdr:colOff>
-          <xdr:row>12</xdr:row>
-          <xdr:rowOff>21614</xdr:rowOff>
+          <xdr:colOff>285750</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>487423</xdr:colOff>
-          <xdr:row>12</xdr:row>
-          <xdr:rowOff>219259</xdr:rowOff>
+          <xdr:colOff>485775</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>219075</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1229,15 +1147,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>281445</xdr:colOff>
-          <xdr:row>13</xdr:row>
-          <xdr:rowOff>128770</xdr:rowOff>
+          <xdr:colOff>292319</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>28247</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>471945</xdr:colOff>
-          <xdr:row>13</xdr:row>
-          <xdr:rowOff>328795</xdr:rowOff>
+          <xdr:colOff>482819</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>228272</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1293,15 +1211,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>275492</xdr:colOff>
-          <xdr:row>14</xdr:row>
-          <xdr:rowOff>16852</xdr:rowOff>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>465992</xdr:colOff>
-          <xdr:row>14</xdr:row>
-          <xdr:rowOff>207352</xdr:rowOff>
+          <xdr:colOff>466725</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1357,22 +1275,22 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>293351</xdr:colOff>
-          <xdr:row>9</xdr:row>
-          <xdr:rowOff>21614</xdr:rowOff>
+          <xdr:colOff>285750</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>483851</xdr:colOff>
-          <xdr:row>9</xdr:row>
-          <xdr:rowOff>219258</xdr:rowOff>
+          <xdr:colOff>476250</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>285750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1050" name="Check Box 26" hidden="1">
+            <xdr:cNvPr id="1053" name="Check Box 29" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1050"/>
+                  <a14:compatExt spid="_x0000_s1053"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1421,86 +1339,22 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>293352</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>27568</xdr:rowOff>
+          <xdr:colOff>283451</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>29888</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>483852</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>225212</xdr:rowOff>
+          <xdr:colOff>483476</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>212177</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1051" name="Check Box 27" hidden="1">
+            <xdr:cNvPr id="1054" name="Check Box 30" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1051"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>286207</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>85909</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>476707</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>285934</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1053" name="Check Box 29" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1053"/>
+                  <a14:compatExt spid="_x0000_s1054"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1748,10 +1602,10 @@
   <sheetPr codeName="Sheet1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1765,17 +1619,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="D1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -1785,404 +1639,361 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
+      <c r="A2" s="22">
         <v>45873</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="21" t="b">
+      <c r="C2" s="15" t="b">
         <v>1</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="18" t="b">
+      <c r="C3" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="15"/>
+      <c r="E3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="10"/>
     </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="9">
+    <row r="4" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="6">
         <v>45812</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="18" t="b">
+      <c r="C4" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="16" t="s">
+      <c r="D4" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="15"/>
+      <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="9">
+      <c r="A5" s="6">
         <v>45812</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="18" t="b">
+      <c r="C5" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="15"/>
+      <c r="E5" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="10"/>
     </row>
     <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="9">
+      <c r="A6" s="6">
         <v>45721</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="18" t="b">
+      <c r="C6" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="15"/>
+      <c r="F6" s="10"/>
     </row>
     <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="18" t="b">
+      <c r="C7" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="15"/>
+      <c r="E7" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="10"/>
     </row>
     <row r="8" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="10"/>
-      <c r="B8" s="3" t="s">
+      <c r="A8" s="7"/>
+      <c r="B8" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="18" t="b">
+      <c r="C8" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="15"/>
+      <c r="D8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
     </row>
     <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10"/>
-      <c r="B9" s="3" t="s">
+      <c r="A9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18" t="b">
+      <c r="C9" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
+      <c r="D9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="10"/>
     </row>
     <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="10"/>
-      <c r="B10" s="3" t="s">
+      <c r="A10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="18" t="b">
+      <c r="C10" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
+      <c r="D10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="10"/>
     </row>
-    <row r="11" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="10"/>
-      <c r="B11" s="3" t="s">
+    <row r="11" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="18" t="b">
+      <c r="C11" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
+      <c r="D11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="10"/>
     </row>
     <row r="12" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="15"/>
+      <c r="F12" s="10"/>
     </row>
-    <row r="13" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="15"/>
-    </row>
-    <row r="14" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="15"/>
+    <row r="13" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="9">
-        <v>45668</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="15"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="12"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="2"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-      <c r="B18" s="17"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="4"/>
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="2"/>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B33:F52 B23:B32 D23:F32">
-    <cfRule type="expression" dxfId="25" priority="38">
-      <formula>$E23=TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18:B20 D18:E20">
-    <cfRule type="expression" dxfId="24" priority="40">
-      <formula>$D18=TRUE</formula>
+  <conditionalFormatting sqref="B20:B29 B30:E49 D20:E29">
+    <cfRule type="expression" dxfId="28" priority="38">
+      <formula>$E20=TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15:B17 D15:E17">
+    <cfRule type="expression" dxfId="27" priority="40">
+      <formula>$D15=TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2 A8:E8">
+    <cfRule type="expression" dxfId="26" priority="55">
+      <formula>#REF!=VERDADEIRO</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10:E10 A7:E7">
+    <cfRule type="expression" dxfId="25" priority="63">
+      <formula>#REF!=VERDADEIRO</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9">
+    <cfRule type="expression" dxfId="24" priority="106">
+      <formula>#REF!=VERDADEIRO</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11:E11">
+    <cfRule type="expression" dxfId="23" priority="30">
+      <formula>#REF!=VERDADEIRO</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12:E12">
+    <cfRule type="expression" dxfId="22" priority="28">
+      <formula>#REF!=VERDADEIRO</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15:B16 D15:E16 A5:E5">
+    <cfRule type="expression" dxfId="21" priority="117">
+      <formula>#REF!=VERDADEIRO</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17:B18 D17:E18">
+    <cfRule type="expression" dxfId="20" priority="18">
+      <formula>$B15=VERDADEIRO</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9 F7">
+    <cfRule type="expression" dxfId="19" priority="19">
+      <formula>#REF!=VERDADEIRO</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10">
+    <cfRule type="expression" dxfId="16" priority="13">
+      <formula>#REF!=VERDADEIRO</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11">
+    <cfRule type="expression" dxfId="15" priority="11">
+      <formula>#REF!=VERDADEIRO</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="expression" dxfId="14" priority="1">
+      <formula>#REF!=VERDADEIRO</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8:D12">
+    <cfRule type="expression" dxfId="13" priority="140">
+      <formula>$B1048559=VERDADEIRO</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7">
+    <cfRule type="expression" dxfId="12" priority="142">
+      <formula>$C30=VERDADEIRO</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="expression" dxfId="11" priority="155">
+      <formula>$C35=VERDADEIRO</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:D12 E2:F7 E8:E12">
+    <cfRule type="expression" dxfId="10" priority="167">
+      <formula>$C2=TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6:F6">
+    <cfRule type="expression" dxfId="9" priority="198">
+      <formula>$D3=VERDADEIRO</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7 A3:F4 F8">
+    <cfRule type="expression" dxfId="7" priority="204">
+      <formula>$D1=VERDADEIRO</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9:C9 F12 E9">
+    <cfRule type="expression" dxfId="6" priority="210">
+      <formula>#REF!=VERDADEIRO</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F20:F49">
+    <cfRule type="expression" dxfId="5" priority="211">
+      <formula>$E20=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1">
-    <cfRule type="expression" dxfId="23" priority="53">
-      <formula>$C1048576=VERDADEIRO</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2">
-    <cfRule type="expression" dxfId="22" priority="55">
-      <formula>#REF!=VERDADEIRO</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9:E9 A13:E13 A7:E7">
-    <cfRule type="expression" dxfId="21" priority="63">
-      <formula>#REF!=VERDADEIRO</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D12">
-    <cfRule type="expression" dxfId="20" priority="106">
-      <formula>#REF!=VERDADEIRO</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14:E14">
-    <cfRule type="expression" dxfId="19" priority="30">
-      <formula>#REF!=VERDADEIRO</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A15:E15">
-    <cfRule type="expression" dxfId="18" priority="28">
-      <formula>#REF!=VERDADEIRO</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18:B19 D18:E19 A10:E11 A5:E5">
-    <cfRule type="expression" dxfId="17" priority="117">
-      <formula>#REF!=VERDADEIRO</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A20:B21 D20:E21">
-    <cfRule type="expression" dxfId="16" priority="18">
-      <formula>$B18=VERDADEIRO</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F9 F13 F7">
-    <cfRule type="expression" dxfId="15" priority="19">
-      <formula>#REF!=VERDADEIRO</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F14">
-    <cfRule type="expression" dxfId="14" priority="15">
-      <formula>#REF!=VERDADEIRO</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F15">
-    <cfRule type="expression" dxfId="13" priority="14">
-      <formula>#REF!=VERDADEIRO</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F10">
-    <cfRule type="expression" dxfId="12" priority="13">
-      <formula>#REF!=VERDADEIRO</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F11">
-    <cfRule type="expression" dxfId="11" priority="11">
-      <formula>#REF!=VERDADEIRO</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
-    <cfRule type="expression" dxfId="10" priority="1">
-      <formula>#REF!=VERDADEIRO</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8:D15">
-    <cfRule type="expression" dxfId="9" priority="140">
-      <formula>$B1048559=VERDADEIRO</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D7">
-    <cfRule type="expression" dxfId="8" priority="142">
-      <formula>$C33=VERDADEIRO</formula>
+    <cfRule type="expression" dxfId="4" priority="215">
+      <formula>$C1048573=VERDADEIRO</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D2">
-    <cfRule type="expression" dxfId="7" priority="154">
-      <formula>$B1048575=VERDADEIRO</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="expression" dxfId="6" priority="155">
-      <formula>$C38=VERDADEIRO</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:C15 E2:F15">
-    <cfRule type="expression" dxfId="5" priority="167">
-      <formula>$C2=TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D15">
-    <cfRule type="expression" dxfId="4" priority="197">
-      <formula>$C2=TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A6:F6">
-    <cfRule type="expression" dxfId="3" priority="198">
-      <formula>$D3=VERDADEIRO</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A15:F15">
-    <cfRule type="expression" dxfId="2" priority="201">
+    <cfRule type="expression" dxfId="3" priority="218">
+      <formula>$B1048572=VERDADEIRO</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11:F12">
+    <cfRule type="expression" dxfId="2" priority="223">
+      <formula>$C8=TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8:F10">
+    <cfRule type="expression" dxfId="1" priority="224">
+      <formula>#REF!=TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12:E12">
+    <cfRule type="expression" dxfId="0" priority="228">
       <formula>$D7=VERDADEIRO</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D7:D8 A3:F4 E8:F8 A8:C8">
-    <cfRule type="expression" dxfId="1" priority="204">
-      <formula>$D1=VERDADEIRO</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E12:F12 A12:C12">
-    <cfRule type="expression" dxfId="0" priority="210">
-      <formula>$D8=VERDADEIRO</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2282,40 +2093,18 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1041" r:id="rId8" name="Check Box 17">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>2</xdr:col>
-                    <xdr:colOff>285750</xdr:colOff>
-                    <xdr:row>7</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>2</xdr:col>
-                    <xdr:colOff>495300</xdr:colOff>
-                    <xdr:row>7</xdr:row>
-                    <xdr:rowOff>219075</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1042" r:id="rId9" name="Check Box 18">
+            <control shapeId="1043" r:id="rId8" name="Check Box 19">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>295275</xdr:colOff>
                     <xdr:row>8</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:rowOff>28575</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:colOff>495300</xdr:colOff>
                     <xdr:row>8</xdr:row>
                     <xdr:rowOff>209550</xdr:rowOff>
                   </to>
@@ -2326,29 +2115,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1043" r:id="rId10" name="Check Box 19">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>2</xdr:col>
-                    <xdr:colOff>295275</xdr:colOff>
-                    <xdr:row>11</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>2</xdr:col>
-                    <xdr:colOff>495300</xdr:colOff>
-                    <xdr:row>11</xdr:row>
-                    <xdr:rowOff>209550</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1045" r:id="rId11" name="Check Box 21">
+            <control shapeId="1045" r:id="rId9" name="Check Box 21">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2370,78 +2137,12 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1046" r:id="rId12" name="Check Box 22">
+            <control shapeId="1046" r:id="rId10" name="Check Box 22">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>285750</xdr:colOff>
-                    <xdr:row>12</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>2</xdr:col>
-                    <xdr:colOff>485775</xdr:colOff>
-                    <xdr:row>12</xdr:row>
-                    <xdr:rowOff>219075</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1048" r:id="rId13" name="Check Box 24">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>2</xdr:col>
-                    <xdr:colOff>285750</xdr:colOff>
-                    <xdr:row>13</xdr:row>
-                    <xdr:rowOff>133350</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>2</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
-                    <xdr:row>13</xdr:row>
-                    <xdr:rowOff>333375</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1049" r:id="rId14" name="Check Box 25">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>2</xdr:col>
-                    <xdr:colOff>276225</xdr:colOff>
-                    <xdr:row>14</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>2</xdr:col>
-                    <xdr:colOff>466725</xdr:colOff>
-                    <xdr:row>14</xdr:row>
-                    <xdr:rowOff>209550</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1050" r:id="rId15" name="Check Box 26">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>2</xdr:col>
-                    <xdr:colOff>295275</xdr:colOff>
                     <xdr:row>9</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </from>
@@ -2458,7 +2159,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1051" r:id="rId16" name="Check Box 27">
+            <control shapeId="1048" r:id="rId11" name="Check Box 24">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2480,7 +2181,29 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1053" r:id="rId17" name="Check Box 29">
+            <control shapeId="1049" r:id="rId12" name="Check Box 25">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>276225</xdr:colOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>466725</xdr:colOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>209550</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1053" r:id="rId13" name="Check Box 29">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2500,6 +2223,28 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1054" r:id="rId14" name="Check Box 30">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>285750</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>209550</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
       </controls>
     </mc:Choice>
   </mc:AlternateContent>

</xml_diff>